<commit_message>
WIP Successor uses gradient - needs different variance
- currently turned off a lot of defaults
- added trail, red for stuck
- going in a straight line causes red, look into
</commit_message>
<xml_diff>
--- a/terrain/Data Collection/Stuck Threshold Data.xlsx
+++ b/terrain/Data Collection/Stuck Threshold Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofsussex-my.sharepoint.com/personal/mb791_sussex_ac_uk/Documents/Third Year/FYP/lizardbot/terrain/Data Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{C2F52F3F-6C71-455F-B81F-0E91038C0D1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{04ACE1C0-FE8C-49F6-BD18-2A34F7ED1111}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{C2F52F3F-6C71-455F-B81F-0E91038C0D1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{223D909E-2B28-48C4-B483-3FF42AFBDF5C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{C7C4BB52-B0D6-4F76-B55F-2BC21352A1C0}"/>
   </bookViews>
@@ -325,7 +325,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
         <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -360,7 +370,19 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{9B2B67E2-F0CF-403F-829D-27E1B233D908}" formatIdx="0">
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-11E1-415D-9490-384408061286}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v>Smooth</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-11E1-415D-9490-384408061286}">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.8</cx:f>
@@ -369,75 +391,23 @@
           </cx:tx>
           <cx:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
           </cx:spPr>
-          <cx:dataLabels>
-            <cx:dataLabel idx="11">
-              <cx:txPr>
-                <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="ctr" rtl="0">
-                    <a:defRPr>
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:r>
-                    <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                    </a:rPr>
-                    <a:t>0.020</a:t>
-                  </a:r>
-                </a:p>
-              </cx:txPr>
-            </cx:dataLabel>
-            <cx:dataLabel idx="12">
-              <cx:txPr>
-                <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="ctr" rtl="0">
-                    <a:defRPr sz="1050" b="1"/>
-                  </a:pPr>
-                  <a:r>
-                    <a:rPr lang="en-US" sz="1050" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                      <a:solidFill>
-                        <a:sysClr val="windowText" lastClr="000000">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:sysClr>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                    </a:rPr>
-                    <a:t>0.023</a:t>
-                  </a:r>
-                </a:p>
-              </cx:txPr>
-            </cx:dataLabel>
-            <cx:dataLabelHidden idx="0"/>
-            <cx:dataLabelHidden idx="9"/>
-            <cx:dataLabelHidden idx="10"/>
-          </cx:dataLabels>
-          <cx:dataId val="0"/>
+          <cx:dataId val="1"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000002-11E1-415D-9490-384408061286}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>Rough</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -1160,7 +1130,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B25B2D14-2766-455C-9013-3C21EFCFE6FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A830921F-67CA-4D8B-9DBF-02DE68A2811D}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -1501,7 +1471,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,13 +1492,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>5.0999999999999997E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C2" s="3">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="D2" s="4">
-        <v>4.7E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1536,13 +1506,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="C3" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D3" s="7">
-        <v>0.22600000000000001</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1550,13 +1520,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>2.7E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C4" s="6">
         <v>0.02</v>
       </c>
       <c r="D4" s="7">
-        <v>0.51500000000000001</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,13 +1534,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>6.3E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="C5" s="6">
         <v>0.01</v>
       </c>
       <c r="D5" s="7">
-        <v>0.39900000000000002</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1578,13 +1548,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>3.1E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="C6" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="D6" s="7">
-        <v>0.31900000000000001</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,13 +1562,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>2.8000000000000001E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C7" s="6">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D7" s="7">
-        <v>0.24299999999999999</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1606,13 +1576,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>6.3E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C8" s="6">
         <v>0.02</v>
       </c>
       <c r="D8" s="7">
-        <v>0.40500000000000003</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1620,13 +1590,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>2.8000000000000001E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="C9" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="D9" s="7">
-        <v>0.30399999999999999</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1634,13 +1604,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C10" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="D10" s="7">
-        <v>0.39</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1648,19 +1618,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="8">
-        <v>6.2E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="C11" s="9">
         <v>1.4E-2</v>
       </c>
       <c r="D11" s="10">
-        <v>0.51100000000000001</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>AVERAGE(B2:B11)</f>
-        <v>3.9000000000000007E-2</v>
+        <v>3.8000000000000004E-3</v>
       </c>
       <c r="C12">
         <f>AVERAGE(C2:C11)</f>
@@ -1668,14 +1638,11 @@
       </c>
       <c r="D12">
         <f>AVERAGE(D2:D11)</f>
-        <v>0.33589999999999998</v>
+        <v>5.8199999999999995E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="1">
-        <f>AVERAGE(B12:D12)</f>
-        <v>0.13146666666666665</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>